<commit_message>
Update main UFC board, to send all segment signals to SCRATCHPAD, COMM1 and COMM2. this will make the software simpler Update main UFC board, POT mounting holes are now first class citizens. Update main UFC board, most layers are filled with ground. in2 is power. Fix main UFC board having isolated grounds. Corrected LED on the 16 segment display binary representation  in UFCconnections.xlsx
</commit_message>
<xml_diff>
--- a/ECAD/PCBs/OH_Specific/Functional/UFCconnections.xlsx
+++ b/ECAD/PCBs/OH_Specific/Functional/UFCconnections.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17790" windowHeight="9720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17790" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MEGA" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="164">
   <si>
     <t>pin</t>
   </si>
@@ -164,9 +164,6 @@
     <t>bit test sw</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>hud bit test</t>
   </si>
   <si>
@@ -329,12 +326,6 @@
     <t>SPI</t>
   </si>
   <si>
-    <t>diode L</t>
-  </si>
-  <si>
-    <t>diode R</t>
-  </si>
-  <si>
     <t>segment</t>
   </si>
   <si>
@@ -425,91 +416,109 @@
     <t>/</t>
   </si>
   <si>
-    <t>0x0010001111000111</t>
-  </si>
-  <si>
-    <t>0x1110100001010010</t>
-  </si>
-  <si>
-    <t>0x1110001001000100</t>
-  </si>
-  <si>
-    <t>0x1110101001000100</t>
-  </si>
-  <si>
-    <t>0x1110101001000000</t>
-  </si>
-  <si>
-    <t>0x0010001111000100</t>
-  </si>
-  <si>
-    <t>0x1100001000000100</t>
-  </si>
-  <si>
-    <t>0x0010000111000000</t>
-  </si>
-  <si>
-    <t>0x0001010000101000</t>
-  </si>
-  <si>
-    <t>0x0001010000100000</t>
-  </si>
-  <si>
-    <t>0x0010011001100100</t>
-  </si>
-  <si>
-    <t>0x0000010000100000</t>
-  </si>
-  <si>
-    <t>0x1100010000100000</t>
-  </si>
-  <si>
-    <t>0x1110001001000111</t>
-  </si>
-  <si>
-    <t>0x1110101001011010</t>
-  </si>
-  <si>
-    <t>0x1110101001010010</t>
-  </si>
-  <si>
-    <t>calculate code for character</t>
-  </si>
-  <si>
-    <t>0x1110001001010101</t>
-  </si>
-  <si>
-    <t>0x1100001000000111</t>
-  </si>
-  <si>
-    <t>0x1101000000100011</t>
-  </si>
-  <si>
-    <t>0x1010101001010101</t>
-  </si>
-  <si>
-    <t>0x1110001001001111</t>
-  </si>
-  <si>
-    <t>0x1100100000011011</t>
-  </si>
-  <si>
-    <t>0x1101000000001011</t>
-  </si>
-  <si>
-    <t>0x0010101111010111</t>
-  </si>
-  <si>
-    <t>0x1100100000101000</t>
-  </si>
-  <si>
-    <t>0x0100001001000111</t>
-  </si>
-  <si>
     <t>w</t>
   </si>
   <si>
-    <t>0x1100010001001011</t>
+    <t>0x0000010000000001</t>
+  </si>
+  <si>
+    <t>0x0100110001001001</t>
+  </si>
+  <si>
+    <t>0x0000010100000101</t>
+  </si>
+  <si>
+    <t>0x0000010100000001</t>
+  </si>
+  <si>
+    <t>0x1001101010011010</t>
+  </si>
+  <si>
+    <t>0x1101100001001000</t>
+  </si>
+  <si>
+    <t>0x1101101001001000</t>
+  </si>
+  <si>
+    <t>0x1101101000001000</t>
+  </si>
+  <si>
+    <t>0x1001001010010010</t>
+  </si>
+  <si>
+    <t>0x0110100011111000</t>
+  </si>
+  <si>
+    <t>0x0110100011111010</t>
+  </si>
+  <si>
+    <t>0x0110100001101000</t>
+  </si>
+  <si>
+    <t>0x0010100000101000</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
+  <si>
+    <t>0x1101100001001100</t>
+  </si>
+  <si>
+    <t>0x1001000110010001</t>
+  </si>
+  <si>
+    <t>0x1001000110010100</t>
+  </si>
+  <si>
+    <t>0x1101000001000000</t>
+  </si>
+  <si>
+    <t>0x1101100011011000</t>
+  </si>
+  <si>
+    <t>0x1101100011011100</t>
+  </si>
+  <si>
+    <t>0x1001101000011110</t>
+  </si>
+  <si>
+    <t>0x1001101000011010</t>
+  </si>
+  <si>
+    <t>0x1100101001011010</t>
+  </si>
+  <si>
+    <t>0x1101000011010000</t>
+  </si>
+  <si>
+    <t>0x1001010000000001</t>
+  </si>
+  <si>
+    <t>0x1001010010010100</t>
+  </si>
+  <si>
+    <t>0x1100000011011000</t>
+  </si>
+  <si>
+    <t>0x1001001000000101</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>code calculated from the left form</t>
+  </si>
+  <si>
+    <t>approx. representation</t>
   </si>
 </sst>
 </file>
@@ -525,7 +534,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -544,6 +553,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -557,13 +578,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,7 +1167,7 @@
         <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
@@ -1160,7 +1184,7 @@
         <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E18" t="s">
         <v>19</v>
@@ -1177,7 +1201,7 @@
         <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E19" t="s">
         <v>19</v>
@@ -1194,10 +1218,10 @@
         <v>44</v>
       </c>
       <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
         <v>45</v>
-      </c>
-      <c r="E20" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1208,13 +1232,13 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" t="s">
         <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1225,13 +1249,13 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
         <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1242,13 +1266,13 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" t="s">
         <v>49</v>
-      </c>
-      <c r="D23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1259,13 +1283,13 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
         <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1276,13 +1300,13 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
         <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1293,13 +1317,13 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26" t="s">
         <v>31</v>
       </c>
       <c r="E26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1310,13 +1334,13 @@
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27" t="s">
         <v>31</v>
       </c>
       <c r="E27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1327,13 +1351,13 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
         <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,13 +1368,13 @@
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
       </c>
       <c r="E29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1361,7 +1385,7 @@
         <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D30" t="s">
         <v>31</v>
@@ -1378,7 +1402,7 @@
         <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D31" t="s">
         <v>31</v>
@@ -1395,7 +1419,7 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D32" t="s">
         <v>31</v>
@@ -1412,7 +1436,7 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D33" t="s">
         <v>31</v>
@@ -1429,7 +1453,7 @@
         <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" t="s">
         <v>31</v>
@@ -1446,7 +1470,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D35" t="s">
         <v>31</v>
@@ -1463,7 +1487,7 @@
         <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D36" t="s">
         <v>31</v>
@@ -1480,7 +1504,7 @@
         <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D37" t="s">
         <v>31</v>
@@ -1497,7 +1521,7 @@
         <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D38" t="s">
         <v>31</v>
@@ -1514,7 +1538,7 @@
         <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D39" t="s">
         <v>31</v>
@@ -1531,13 +1555,13 @@
         <v>40</v>
       </c>
       <c r="C40" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" t="s">
         <v>67</v>
-      </c>
-      <c r="D40" t="s">
-        <v>31</v>
-      </c>
-      <c r="E40" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1548,13 +1572,13 @@
         <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D41" t="s">
         <v>31</v>
       </c>
       <c r="E41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1565,13 +1589,13 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1582,13 +1606,13 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1599,13 +1623,13 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1616,13 +1640,13 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1633,13 +1657,13 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1650,13 +1674,13 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1667,13 +1691,13 @@
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1684,13 +1708,13 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1701,13 +1725,13 @@
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1764,138 +1788,138 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
         <v>81</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>82</v>
       </c>
-      <c r="C2" t="s">
-        <v>83</v>
-      </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" t="s">
         <v>94</v>
       </c>
-      <c r="C8" t="s">
-        <v>95</v>
-      </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" t="s">
         <v>96</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>97</v>
       </c>
-      <c r="D9" t="s">
-        <v>98</v>
-      </c>
       <c r="E9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1905,10 +1929,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1916,187 +1940,196 @@
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="4" width="3.42578125" customWidth="1"/>
     <col min="5" max="5" width="3.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" customWidth="1"/>
+    <col min="12" max="18" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="T1" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="C2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="4">
+        <v>2</v>
+      </c>
+      <c r="I2" s="4">
+        <v>16</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="T2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="4">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4">
+        <v>14</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="T3" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="4">
+        <v>8</v>
+      </c>
+      <c r="I4" s="4">
+        <v>9</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="T4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3">
+      <c r="D5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="4">
         <v>1</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I5" s="4">
         <v>15</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3" t="s">
+      <c r="K5" s="4"/>
+      <c r="T5" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H6" s="4">
+        <v>3</v>
+      </c>
+      <c r="I6" s="4">
+        <v>10</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="T6" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3">
-        <v>2</v>
-      </c>
-      <c r="I4" s="3">
-        <v>16</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3">
-        <v>3</v>
-      </c>
-      <c r="I5" s="3">
-        <v>10</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G6" s="3"/>
-      <c r="H6" s="3">
-        <v>4</v>
-      </c>
-      <c r="I6" s="3">
-        <v>11</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="U6" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
       <c r="D7" s="2">
         <v>10</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3">
-        <v>5</v>
-      </c>
-      <c r="I7" s="3">
-        <v>12</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G7" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H7" s="4">
+        <v>6</v>
+      </c>
+      <c r="I7" s="4">
+        <v>13</v>
+      </c>
+      <c r="K7" s="4"/>
+      <c r="T7" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -2112,50 +2145,48 @@
       <c r="E8" s="2">
         <v>15</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3">
-        <v>6</v>
-      </c>
-      <c r="I8" s="3">
-        <v>13</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G8" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="4">
+        <v>5</v>
+      </c>
+      <c r="I8" s="4">
+        <v>12</v>
+      </c>
+      <c r="K8" s="4"/>
+      <c r="T8" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="U8" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
       <c r="D9" s="2">
         <v>12</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3">
-        <v>7</v>
-      </c>
-      <c r="I9" s="3">
-        <v>14</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9" s="4">
+        <v>4</v>
+      </c>
+      <c r="I9" s="4">
+        <v>11</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="T9" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="U9" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -2171,74 +2202,94 @@
       <c r="E10" s="2">
         <v>16</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3">
-        <v>8</v>
-      </c>
-      <c r="I10" s="3">
-        <v>9</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="T10" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="U10" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>7</v>
       </c>
       <c r="D11" s="2">
         <v>14</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="M12" s="5" t="s">
+      <c r="G11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="T11" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="U11" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" t="s">
+        <v>163</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="U12" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>145</v>
+      </c>
       <c r="B13" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>143</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E13" t="str">
+        <f>"/"</f>
+        <v>/</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="K13" s="4"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="8" t="str">
+        <f>IF(B13=1,"*","")</f>
+        <v>*</v>
+      </c>
+      <c r="N13" s="8" t="str">
+        <f>IF(B13=1,"*","")</f>
+        <v>*</v>
+      </c>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8" t="str">
+        <f>IF(D13=1,"*","")</f>
+        <v>*</v>
+      </c>
+      <c r="Q13" s="8" t="str">
+        <f>IF(D13=1,"*","")</f>
+        <v>*</v>
+      </c>
+      <c r="R13" s="8"/>
+      <c r="T13" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="U13" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -2247,42 +2298,92 @@
         <v>0</v>
       </c>
       <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
         <v>0</v>
       </c>
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
-      <c r="G14" s="3" t="str">
-        <f>CONCATENATE("0x",A14,A16,B13,B14,B15,B16,B17,C14,C16,D13,D14,D15,D16,D17,E14,E16)</f>
-        <v>0x1100010001001011</v>
-      </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G14" s="4" t="str">
+        <f>CONCATENATE("0x",A16,B17,C14,A14,B13,B16,B15,B14,E16,D17,C16,E14,D13,D16,D15,D14)</f>
+        <v>0x0100110001001001</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="L14" s="8" t="str">
+        <f>IF(A14=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="M14" s="8" t="str">
+        <f>IF(B14=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8" t="str">
+        <f>IF(C14=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8" t="str">
+        <f>IF(D14=1,"*","")</f>
+        <v>*</v>
+      </c>
+      <c r="R14" s="8" t="str">
+        <f>IF(E14=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="U14" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>144</v>
+      </c>
       <c r="B15" s="1">
         <v>0</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="M15" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>144</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="8" t="str">
+        <f>IF(A14=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8" t="str">
+        <f>IF(B14=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="O15" s="8" t="str">
+        <f>IF(C14=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="P15" s="8" t="str">
+        <f>IF(D14=1,"*","")</f>
+        <v>*</v>
+      </c>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8" t="str">
+        <f>IF(E14=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="U15" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -2291,132 +2392,216 @@
         <v>0</v>
       </c>
       <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8" t="str">
+        <f>IF(B15=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="N16" s="8" t="str">
+        <f>IF(B15=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8" t="str">
+        <f>IF(D15=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="Q16" s="8" t="str">
+        <f>IF(D15=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="R16" s="8"/>
+      <c r="T16" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U16" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>"/"</f>
+        <v>/</v>
+      </c>
+      <c r="B17" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="2">
+      <c r="C17" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" s="2">
         <v>1</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3" t="s">
+      <c r="E17" t="s">
+        <v>145</v>
+      </c>
+      <c r="L17" s="8" t="str">
+        <f>IF(A16=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8" t="str">
+        <f>IF(B16=1,"*","")</f>
+        <v>*</v>
+      </c>
+      <c r="O17" s="8" t="str">
+        <f>IF(C16=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="P17" s="8" t="str">
+        <f>IF(D16=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8" t="str">
+        <f>IF(E16=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="U17" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L18" s="8" t="str">
+        <f>IF(A16=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="M18" s="8" t="str">
+        <f>IF(B16=1,"*","")</f>
+        <v>*</v>
+      </c>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8" t="str">
+        <f>IF(C16=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8" t="str">
+        <f>IF(D16=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="R18" s="8" t="str">
+        <f>IF(E16=1,"*","")</f>
+        <v/>
+      </c>
+      <c r="T18" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="U18" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L19" s="8"/>
+      <c r="M19" s="8" t="str">
+        <f>IF(B17=1,"*","")</f>
+        <v>*</v>
+      </c>
+      <c r="N19" s="8" t="str">
+        <f>IF(B17=1,"*","")</f>
+        <v>*</v>
+      </c>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8" t="str">
+        <f>IF(D17=1,"*","")</f>
+        <v>*</v>
+      </c>
+      <c r="Q19" s="8" t="str">
+        <f>IF(D17=1,"*","")</f>
+        <v>*</v>
+      </c>
+      <c r="R19" s="8"/>
+      <c r="T19" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="U19" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T20" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="U20" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T21" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="U21" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T22" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="U22" s="6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L18" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L19" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L20" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="M20" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L21" s="3" t="s">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T23" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="M21" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L22" s="3" t="s">
+      <c r="U23" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T24" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="U24" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T25" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="M22" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L23" s="3" t="s">
+      <c r="U25" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T26" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="M23" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L24" s="3" t="s">
+      <c r="U26" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T27" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="M24" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L25" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L26" s="3" t="s">
+      <c r="U27" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T28" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="M26" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L27" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L28" s="3" t="s">
+      <c r="U28" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="M28" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L29" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="M29" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L30" s="3"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L30" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'ABSIS_2.0' of https://github.com/jrsteensen/OpenHornet into ABSIS_2.0"
This reverts commit cac173c4110ad9f0d1ad5a88a6b4048d6b756427, reversing
changes made to d0a675c2168bb1c3cb62f6e4a84cc7e34bb45d3d.
</commit_message>
<xml_diff>
--- a/ECAD/PCBs/OH_Specific/Functional/UFCconnections.xlsx
+++ b/ECAD/PCBs/OH_Specific/Functional/UFCconnections.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17790" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17790" windowHeight="9720"/>
   </bookViews>
   <sheets>
     <sheet name="MEGA" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="161">
   <si>
     <t>pin</t>
   </si>
@@ -164,6 +164,9 @@
     <t>bit test sw</t>
   </si>
   <si>
+    <t>?</t>
+  </si>
+  <si>
     <t>hud bit test</t>
   </si>
   <si>
@@ -326,6 +329,12 @@
     <t>SPI</t>
   </si>
   <si>
+    <t>diode L</t>
+  </si>
+  <si>
+    <t>diode R</t>
+  </si>
+  <si>
     <t>segment</t>
   </si>
   <si>
@@ -416,109 +425,91 @@
     <t>/</t>
   </si>
   <si>
+    <t>0x0010001111000111</t>
+  </si>
+  <si>
+    <t>0x1110100001010010</t>
+  </si>
+  <si>
+    <t>0x1110001001000100</t>
+  </si>
+  <si>
+    <t>0x1110101001000100</t>
+  </si>
+  <si>
+    <t>0x1110101001000000</t>
+  </si>
+  <si>
+    <t>0x0010001111000100</t>
+  </si>
+  <si>
+    <t>0x1100001000000100</t>
+  </si>
+  <si>
+    <t>0x0010000111000000</t>
+  </si>
+  <si>
+    <t>0x0001010000101000</t>
+  </si>
+  <si>
+    <t>0x0001010000100000</t>
+  </si>
+  <si>
+    <t>0x0010011001100100</t>
+  </si>
+  <si>
+    <t>0x0000010000100000</t>
+  </si>
+  <si>
+    <t>0x1100010000100000</t>
+  </si>
+  <si>
+    <t>0x1110001001000111</t>
+  </si>
+  <si>
+    <t>0x1110101001011010</t>
+  </si>
+  <si>
+    <t>0x1110101001010010</t>
+  </si>
+  <si>
+    <t>calculate code for character</t>
+  </si>
+  <si>
+    <t>0x1110001001010101</t>
+  </si>
+  <si>
+    <t>0x1100001000000111</t>
+  </si>
+  <si>
+    <t>0x1101000000100011</t>
+  </si>
+  <si>
+    <t>0x1010101001010101</t>
+  </si>
+  <si>
+    <t>0x1110001001001111</t>
+  </si>
+  <si>
+    <t>0x1100100000011011</t>
+  </si>
+  <si>
+    <t>0x1101000000001011</t>
+  </si>
+  <si>
+    <t>0x0010101111010111</t>
+  </si>
+  <si>
+    <t>0x1100100000101000</t>
+  </si>
+  <si>
+    <t>0x0100001001000111</t>
+  </si>
+  <si>
     <t>w</t>
   </si>
   <si>
-    <t>0x0000010000000001</t>
-  </si>
-  <si>
-    <t>0x0100110001001001</t>
-  </si>
-  <si>
-    <t>0x0000010100000101</t>
-  </si>
-  <si>
-    <t>0x0000010100000001</t>
-  </si>
-  <si>
-    <t>0x1001101010011010</t>
-  </si>
-  <si>
-    <t>0x1101100001001000</t>
-  </si>
-  <si>
-    <t>0x1101101001001000</t>
-  </si>
-  <si>
-    <t>0x1101101000001000</t>
-  </si>
-  <si>
-    <t>0x1001001010010010</t>
-  </si>
-  <si>
-    <t>0x0110100011111000</t>
-  </si>
-  <si>
-    <t>0x0110100011111010</t>
-  </si>
-  <si>
-    <t>0x0110100001101000</t>
-  </si>
-  <si>
-    <t>0x0010100000101000</t>
-  </si>
-  <si>
-    <t>|</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>\</t>
-  </si>
-  <si>
-    <t>0x1101100001001100</t>
-  </si>
-  <si>
-    <t>0x1001000110010001</t>
-  </si>
-  <si>
-    <t>0x1001000110010100</t>
-  </si>
-  <si>
-    <t>0x1101000001000000</t>
-  </si>
-  <si>
-    <t>0x1101100011011000</t>
-  </si>
-  <si>
-    <t>0x1101100011011100</t>
-  </si>
-  <si>
-    <t>0x1001101000011110</t>
-  </si>
-  <si>
-    <t>0x1001101000011010</t>
-  </si>
-  <si>
-    <t>0x1100101001011010</t>
-  </si>
-  <si>
-    <t>0x1101000011010000</t>
-  </si>
-  <si>
-    <t>0x1001010000000001</t>
-  </si>
-  <si>
-    <t>0x1001010010010100</t>
-  </si>
-  <si>
-    <t>0x1100000011011000</t>
-  </si>
-  <si>
-    <t>0x1001001000000101</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>code calculated from the left form</t>
-  </si>
-  <si>
-    <t>approx. representation</t>
+    <t>0x1100010001001011</t>
   </si>
 </sst>
 </file>
@@ -534,7 +525,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -553,18 +544,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -578,16 +557,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1143,7 @@
         <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
@@ -1184,7 +1160,7 @@
         <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E18" t="s">
         <v>19</v>
@@ -1201,7 +1177,7 @@
         <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E19" t="s">
         <v>19</v>
@@ -1218,10 +1194,10 @@
         <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1232,13 +1208,13 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
         <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1249,13 +1225,13 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D22" t="s">
         <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1266,13 +1242,13 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s">
         <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1283,13 +1259,13 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" t="s">
         <v>50</v>
-      </c>
-      <c r="D24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1300,13 +1276,13 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
         <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1317,13 +1293,13 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s">
         <v>31</v>
       </c>
       <c r="E26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1334,13 +1310,13 @@
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
         <v>31</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1351,13 +1327,13 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D28" t="s">
         <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1368,13 +1344,13 @@
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
       </c>
       <c r="E29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1385,7 +1361,7 @@
         <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D30" t="s">
         <v>31</v>
@@ -1402,7 +1378,7 @@
         <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D31" t="s">
         <v>31</v>
@@ -1419,7 +1395,7 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s">
         <v>31</v>
@@ -1436,7 +1412,7 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D33" t="s">
         <v>31</v>
@@ -1453,7 +1429,7 @@
         <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D34" t="s">
         <v>31</v>
@@ -1470,7 +1446,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D35" t="s">
         <v>31</v>
@@ -1487,7 +1463,7 @@
         <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D36" t="s">
         <v>31</v>
@@ -1504,7 +1480,7 @@
         <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D37" t="s">
         <v>31</v>
@@ -1521,7 +1497,7 @@
         <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D38" t="s">
         <v>31</v>
@@ -1538,7 +1514,7 @@
         <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D39" t="s">
         <v>31</v>
@@ -1555,13 +1531,13 @@
         <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D40" t="s">
         <v>31</v>
       </c>
       <c r="E40" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1572,13 +1548,13 @@
         <v>38</v>
       </c>
       <c r="C41" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" t="s">
         <v>68</v>
-      </c>
-      <c r="D41" t="s">
-        <v>31</v>
-      </c>
-      <c r="E41" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1589,13 +1565,13 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E42" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1606,13 +1582,13 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D43" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E43" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1623,13 +1599,13 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
+        <v>71</v>
+      </c>
+      <c r="D44" t="s">
         <v>70</v>
       </c>
-      <c r="D44" t="s">
-        <v>69</v>
-      </c>
       <c r="E44" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1640,13 +1616,13 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D45" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E45" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1657,13 +1633,13 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D46" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E46" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1674,13 +1650,13 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D47" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E47" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1691,13 +1667,13 @@
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D48" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1708,13 +1684,13 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D49" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E49" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1725,13 +1701,13 @@
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D50" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E50" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1788,138 +1764,138 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" t="s">
         <v>80</v>
-      </c>
-      <c r="B2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" t="s">
         <v>80</v>
-      </c>
-      <c r="B3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" t="s">
         <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" t="s">
         <v>80</v>
-      </c>
-      <c r="B5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
         <v>80</v>
-      </c>
-      <c r="B6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" t="s">
         <v>80</v>
-      </c>
-      <c r="B7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" t="s">
         <v>80</v>
-      </c>
-      <c r="B8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" t="s">
         <v>80</v>
-      </c>
-      <c r="B9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1929,10 +1905,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,196 +1916,187 @@
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="4" width="3.42578125" customWidth="1"/>
     <col min="5" max="5" width="3.140625" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" customWidth="1"/>
-    <col min="10" max="10" width="4.140625" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" customWidth="1"/>
-    <col min="12" max="18" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>15</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="T1" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="U1" s="4" t="s">
+      <c r="E4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3">
+        <v>16</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3">
+        <v>3</v>
+      </c>
+      <c r="I5" s="3">
+        <v>10</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3">
+        <v>4</v>
+      </c>
+      <c r="I6" s="3">
+        <v>11</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="H2" s="4">
-        <v>2</v>
-      </c>
-      <c r="I2" s="4">
-        <v>16</v>
-      </c>
-      <c r="K2" s="4"/>
-      <c r="T2" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" s="4">
-        <v>7</v>
-      </c>
-      <c r="I3" s="4">
-        <v>14</v>
-      </c>
-      <c r="K3" s="4"/>
-      <c r="T3" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" s="4">
-        <v>8</v>
-      </c>
-      <c r="I4" s="4">
-        <v>9</v>
-      </c>
-      <c r="K4" s="4"/>
-      <c r="T4" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1</v>
-      </c>
-      <c r="I5" s="4">
-        <v>15</v>
-      </c>
-      <c r="K5" s="4"/>
-      <c r="T5" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="G6" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="H6" s="4">
-        <v>3</v>
-      </c>
-      <c r="I6" s="4">
-        <v>10</v>
-      </c>
-      <c r="K6" s="4"/>
-      <c r="T6" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="U6" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K6" s="3"/>
+      <c r="L6" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
       <c r="D7" s="2">
         <v>10</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="H7" s="4">
-        <v>6</v>
-      </c>
-      <c r="I7" s="4">
-        <v>13</v>
-      </c>
-      <c r="K7" s="4"/>
-      <c r="T7" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3">
+        <v>5</v>
+      </c>
+      <c r="I7" s="3">
+        <v>12</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -2145,48 +2112,50 @@
       <c r="E8" s="2">
         <v>15</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="H8" s="4">
-        <v>5</v>
-      </c>
-      <c r="I8" s="4">
-        <v>12</v>
-      </c>
-      <c r="K8" s="4"/>
-      <c r="T8" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="U8" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3">
+        <v>6</v>
+      </c>
+      <c r="I8" s="3">
+        <v>13</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
       <c r="D9" s="2">
         <v>12</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H9" s="4">
-        <v>4</v>
-      </c>
-      <c r="I9" s="4">
-        <v>11</v>
-      </c>
-      <c r="K9" s="4"/>
-      <c r="T9" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="U9" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G9" s="3"/>
+      <c r="H9" s="3">
+        <v>7</v>
+      </c>
+      <c r="I9" s="3">
+        <v>14</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -2202,94 +2171,74 @@
       <c r="E10" s="2">
         <v>16</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="T10" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="U10" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3">
+        <v>8</v>
+      </c>
+      <c r="I10" s="3">
+        <v>9</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>7</v>
       </c>
       <c r="D11" s="2">
         <v>14</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="T11" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="U11" s="6" t="s">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="M12" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="G12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" t="s">
-        <v>163</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="U12" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>145</v>
-      </c>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>143</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
-      <c r="E13" t="str">
-        <f>"/"</f>
-        <v>/</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="K13" s="4"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="8" t="str">
-        <f>IF(B13=1,"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="N13" s="8" t="str">
-        <f>IF(B13=1,"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8" t="str">
-        <f>IF(D13=1,"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="Q13" s="8" t="str">
-        <f>IF(D13=1,"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="R13" s="8"/>
-      <c r="T13" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="U13" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -2298,92 +2247,42 @@
         <v>0</v>
       </c>
       <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
         <v>1</v>
       </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="4" t="str">
-        <f>CONCATENATE("0x",A16,B17,C14,A14,B13,B16,B15,B14,E16,D17,C16,E14,D13,D16,D15,D14)</f>
-        <v>0x0100110001001001</v>
-      </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="8" t="str">
-        <f>IF(A14=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="M14" s="8" t="str">
-        <f>IF(B14=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8" t="str">
-        <f>IF(C14=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8" t="str">
-        <f>IF(D14=1,"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="R14" s="8" t="str">
-        <f>IF(E14=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="T14" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="U14" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>144</v>
-      </c>
+      <c r="G14" s="3" t="str">
+        <f>CONCATENATE("0x",A14,A16,B13,B14,B15,B16,B17,C14,C16,D13,D14,D15,D16,D17,E14,E16)</f>
+        <v>0x1100010001001011</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>0</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
-        <v>144</v>
-      </c>
-      <c r="G15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="8" t="str">
-        <f>IF(A14=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8" t="str">
-        <f>IF(B14=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="O15" s="8" t="str">
-        <f>IF(C14=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="P15" s="8" t="str">
-        <f>IF(D14=1,"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8" t="str">
-        <f>IF(E14=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="T15" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="U15" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -2392,216 +2291,132 @@
         <v>0</v>
       </c>
       <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
         <v>0</v>
       </c>
-      <c r="E16" s="2">
+      <c r="D17" s="2">
         <v>0</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8" t="str">
-        <f>IF(B15=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="N16" s="8" t="str">
-        <f>IF(B15=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8" t="str">
-        <f>IF(D15=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="Q16" s="8" t="str">
-        <f>IF(D15=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="R16" s="8"/>
-      <c r="T16" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="U16" s="6" t="s">
+      <c r="L17" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L18" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L19" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L20" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L21" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L22" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L23" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="M23" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
-        <f>"/"</f>
-        <v>/</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L24" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L25" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L26" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L27" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L28" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L29" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="M29" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D17" s="2">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>145</v>
-      </c>
-      <c r="L17" s="8" t="str">
-        <f>IF(A16=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8" t="str">
-        <f>IF(B16=1,"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="O17" s="8" t="str">
-        <f>IF(C16=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="P17" s="8" t="str">
-        <f>IF(D16=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8" t="str">
-        <f>IF(E16=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="T17" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="U17" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="L18" s="8" t="str">
-        <f>IF(A16=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="M18" s="8" t="str">
-        <f>IF(B16=1,"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8" t="str">
-        <f>IF(C16=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8" t="str">
-        <f>IF(D16=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="R18" s="8" t="str">
-        <f>IF(E16=1,"*","")</f>
-        <v/>
-      </c>
-      <c r="T18" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="U18" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="L19" s="8"/>
-      <c r="M19" s="8" t="str">
-        <f>IF(B17=1,"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="N19" s="8" t="str">
-        <f>IF(B17=1,"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8" t="str">
-        <f>IF(D17=1,"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="Q19" s="8" t="str">
-        <f>IF(D17=1,"*","")</f>
-        <v>*</v>
-      </c>
-      <c r="R19" s="8"/>
-      <c r="T19" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="U19" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T20" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="U20" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T21" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="U21" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T22" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="U22" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T23" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="U23" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T24" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="U24" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T25" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="U25" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T26" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="U26" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T27" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="U27" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="T28" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="U28" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="L30" s="4"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated PCBs to use 0.45mm/0.2mm vias updated gerber files for all modified boards. added panelzed gerber files
</commit_message>
<xml_diff>
--- a/ECAD/PCBs/OH_Specific/Functional/UFCconnections.xlsx
+++ b/ECAD/PCBs/OH_Specific/Functional/UFCconnections.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17790" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17790" windowHeight="6735" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="MEGA" sheetId="1" r:id="rId1"/>
+    <sheet name="UFC controller" sheetId="1" r:id="rId1"/>
     <sheet name="key matrix" sheetId="4" r:id="rId2"/>
     <sheet name="backlight" sheetId="2" r:id="rId3"/>
     <sheet name="16-seg dot matrix" sheetId="3" r:id="rId4"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="165">
   <si>
     <t>pin</t>
   </si>
@@ -83,9 +83,6 @@
     <t>chip</t>
   </si>
   <si>
-    <t>mega</t>
-  </si>
-  <si>
     <t>max7219</t>
   </si>
   <si>
@@ -519,6 +516,12 @@
   </si>
   <si>
     <t>approx. representation</t>
+  </si>
+  <si>
+    <t>board</t>
+  </si>
+  <si>
+    <t>UFC controller</t>
   </si>
 </sst>
 </file>
@@ -871,7 +874,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="A2" sqref="A2:A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,7 +889,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -895,843 +898,843 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B17">
         <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B18">
         <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B19">
         <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
         <v>44</v>
-      </c>
-      <c r="D20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B21">
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B22">
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
         <v>48</v>
-      </c>
-      <c r="D23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B24">
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B25">
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B26">
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B27">
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B28">
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B29">
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B30">
         <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B31">
         <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B32">
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B33">
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B34">
         <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B35">
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B36">
         <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B37">
         <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B38">
         <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B39">
         <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B40">
         <v>40</v>
       </c>
       <c r="C40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" t="s">
         <v>66</v>
-      </c>
-      <c r="D40" t="s">
-        <v>31</v>
-      </c>
-      <c r="E40" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B41">
         <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B42">
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B43">
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B44">
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B45">
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B46">
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B47">
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B48">
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B49">
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="B50">
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1758,7 +1761,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,146 +1783,146 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
         <v>80</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>81</v>
       </c>
-      <c r="C2" t="s">
-        <v>82</v>
-      </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" t="s">
         <v>93</v>
       </c>
-      <c r="C8" t="s">
-        <v>94</v>
-      </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" t="s">
         <v>95</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>96</v>
       </c>
-      <c r="D9" t="s">
-        <v>97</v>
-      </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1932,7 +1935,7 @@
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,47 +1953,47 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>161</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="T1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="G2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H2" s="4">
         <v>2</v>
@@ -2000,21 +2003,21 @@
       </c>
       <c r="K2" s="4"/>
       <c r="T2" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
@@ -2024,30 +2027,30 @@
       </c>
       <c r="K3" s="4"/>
       <c r="T3" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" s="4">
         <v>8</v>
@@ -2057,21 +2060,21 @@
       </c>
       <c r="K4" s="4"/>
       <c r="T4" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H5" s="4">
         <v>1</v>
@@ -2081,15 +2084,15 @@
       </c>
       <c r="K5" s="4"/>
       <c r="T5" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U5" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G6" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H6" s="4">
         <v>3</v>
@@ -2099,10 +2102,10 @@
       </c>
       <c r="K6" s="4"/>
       <c r="T6" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -2113,7 +2116,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H7" s="4">
         <v>6</v>
@@ -2123,10 +2126,10 @@
       </c>
       <c r="K7" s="4"/>
       <c r="T7" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -2146,7 +2149,7 @@
         <v>15</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H8" s="4">
         <v>5</v>
@@ -2156,10 +2159,10 @@
       </c>
       <c r="K8" s="4"/>
       <c r="T8" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="U8" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -2170,7 +2173,7 @@
         <v>12</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H9" s="4">
         <v>4</v>
@@ -2180,10 +2183,10 @@
       </c>
       <c r="K9" s="4"/>
       <c r="T9" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="U9" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -2205,10 +2208,10 @@
       <c r="G10" s="4"/>
       <c r="K10" s="4"/>
       <c r="T10" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="U10" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -2221,70 +2224,70 @@
       <c r="G11" s="4"/>
       <c r="K11" s="4"/>
       <c r="T11" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U11" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U12" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="str">
         <f>"/"</f>
         <v>/</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="7"/>
       <c r="M13" s="8" t="str">
         <f>IF(B13=1,"*","")</f>
-        <v>*</v>
+        <v/>
       </c>
       <c r="N13" s="8" t="str">
         <f>IF(B13=1,"*","")</f>
-        <v>*</v>
+        <v/>
       </c>
       <c r="O13" s="8"/>
       <c r="P13" s="8" t="str">
         <f>IF(D13=1,"*","")</f>
-        <v>*</v>
+        <v/>
       </c>
       <c r="Q13" s="8" t="str">
         <f>IF(D13=1,"*","")</f>
-        <v>*</v>
+        <v/>
       </c>
       <c r="R13" s="8"/>
       <c r="T13" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U13" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2295,17 +2298,17 @@
         <v>0</v>
       </c>
       <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
         <v>0</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1</v>
       </c>
       <c r="E14" s="2">
         <v>0</v>
       </c>
       <c r="G14" s="4" t="str">
         <f>CONCATENATE("0x",A16,B17,C14,A14,B13,B16,B15,B14,E16,D17,C16,E14,D13,D16,D15,D14)</f>
-        <v>0x0100110001001001</v>
+        <v>0x0010000000100000</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="8" t="str">
@@ -2319,27 +2322,27 @@
       <c r="N14" s="8"/>
       <c r="O14" s="8" t="str">
         <f>IF(C14=1,"*","")</f>
-        <v/>
+        <v>*</v>
       </c>
       <c r="P14" s="8"/>
       <c r="Q14" s="8" t="str">
         <f>IF(D14=1,"*","")</f>
-        <v>*</v>
+        <v/>
       </c>
       <c r="R14" s="8" t="str">
         <f>IF(E14=1,"*","")</f>
         <v/>
       </c>
       <c r="T14" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -2348,7 +2351,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G15" s="4"/>
       <c r="K15" s="4"/>
@@ -2363,11 +2366,11 @@
       </c>
       <c r="O15" s="8" t="str">
         <f>IF(C14=1,"*","")</f>
-        <v/>
+        <v>*</v>
       </c>
       <c r="P15" s="8" t="str">
         <f>IF(D14=1,"*","")</f>
-        <v>*</v>
+        <v/>
       </c>
       <c r="Q15" s="8"/>
       <c r="R15" s="8" t="str">
@@ -2375,10 +2378,10 @@
         <v/>
       </c>
       <c r="T15" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="U15" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2386,10 +2389,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
         <v>1</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
@@ -2419,10 +2422,10 @@
       </c>
       <c r="R16" s="8"/>
       <c r="T16" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U16" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2431,16 +2434,16 @@
         <v>/</v>
       </c>
       <c r="B17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L17" s="8" t="str">
         <f>IF(A16=1,"*","")</f>
@@ -2449,11 +2452,11 @@
       <c r="M17" s="8"/>
       <c r="N17" s="8" t="str">
         <f>IF(B16=1,"*","")</f>
-        <v>*</v>
+        <v/>
       </c>
       <c r="O17" s="8" t="str">
         <f>IF(C16=1,"*","")</f>
-        <v/>
+        <v>*</v>
       </c>
       <c r="P17" s="8" t="str">
         <f>IF(D16=1,"*","")</f>
@@ -2465,10 +2468,10 @@
         <v/>
       </c>
       <c r="T17" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U17" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -2478,12 +2481,12 @@
       </c>
       <c r="M18" s="8" t="str">
         <f>IF(B16=1,"*","")</f>
-        <v>*</v>
+        <v/>
       </c>
       <c r="N18" s="8"/>
       <c r="O18" s="8" t="str">
         <f>IF(C16=1,"*","")</f>
-        <v/>
+        <v>*</v>
       </c>
       <c r="P18" s="8"/>
       <c r="Q18" s="8" t="str">
@@ -2495,109 +2498,109 @@
         <v/>
       </c>
       <c r="T18" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U18" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L19" s="8"/>
       <c r="M19" s="8" t="str">
         <f>IF(B17=1,"*","")</f>
-        <v>*</v>
+        <v/>
       </c>
       <c r="N19" s="8" t="str">
         <f>IF(B17=1,"*","")</f>
-        <v>*</v>
+        <v/>
       </c>
       <c r="O19" s="8"/>
       <c r="P19" s="8" t="str">
         <f>IF(D17=1,"*","")</f>
-        <v>*</v>
+        <v/>
       </c>
       <c r="Q19" s="8" t="str">
         <f>IF(D17=1,"*","")</f>
-        <v>*</v>
+        <v/>
       </c>
       <c r="R19" s="8"/>
       <c r="T19" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="U19" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T20" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="U20" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T21" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U21" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T22" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U22" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T23" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="U23" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T24" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U24" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T25" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U25" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T26" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U26" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T27" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="U27" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T28" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U28" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>